<commit_message>
Added SDSTestCases.xlsx for the test case excel.
Included the SDSTestCases.xlsx sheet which contains our 10 test cases.
</commit_message>
<xml_diff>
--- a/SDSTestCases.xlsx
+++ b/SDSTestCases.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27511"/>
-  <workbookPr/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10211"/>
+  <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://sdsuedu-my.sharepoint.com/personal/rsivaraj0153_sdsu_edu/Documents/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rithishsivaraj/Desktop/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{F16F1ABD-2D39-444E-8116-1781F6AF9AC4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{0B04F18E-675C-1E42-9046-EE6AA4D7E931}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1100" yWindow="820" windowWidth="28040" windowHeight="17440" xr2:uid="{FA00CF0B-2032-3346-BC09-3481BA2E6547}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191028"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="76">
   <si>
     <t>TestCaseId</t>
   </si>
@@ -83,9 +83,21 @@
     <t>Site is already open</t>
   </si>
   <si>
+    <t>AddMovie_1</t>
+  </si>
+  <si>
     <t>1. Search bar is clicked on site.</t>
   </si>
   <si>
+    <t>Admin_Database_Edit</t>
+  </si>
+  <si>
+    <t>Verify that Administrative users can add to movie database</t>
+  </si>
+  <si>
+    <t>Admin account logged in</t>
+  </si>
+  <si>
     <t>Movies relating to "titanic are displayed</t>
   </si>
   <si>
@@ -98,16 +110,16 @@
     <t>TesterRithish</t>
   </si>
   <si>
-    <t>AddMovie_1</t>
-  </si>
-  <si>
-    <t>Admin_Database_Edit</t>
-  </si>
-  <si>
-    <t>Verify that Administrative users can add to movie database</t>
-  </si>
-  <si>
-    <t>Admin account logged in</t>
+    <t>SeatSelect_1</t>
+  </si>
+  <si>
+    <t>Seat_Select_Booking</t>
+  </si>
+  <si>
+    <t>P4</t>
+  </si>
+  <si>
+    <t>Verify that seats can be selected without double booking.</t>
   </si>
   <si>
     <t>1. Navigate to user page.  
@@ -120,6 +132,9 @@
 6. Search in the site's movie search bar for the added movie's name.</t>
   </si>
   <si>
+    <t>Movie should be chosen and should be on booking page.</t>
+  </si>
+  <si>
     <t>Newly-added movie listing appears, and 
 has an associated page with added 
 information.</t>
@@ -132,24 +147,10 @@
     <t>TesterPotter</t>
   </si>
   <si>
-    <t>SeatSelect_1</t>
-  </si>
-  <si>
-    <t>Seat_Select_Booking</t>
-  </si>
-  <si>
-    <t>P4</t>
-  </si>
-  <si>
-    <t>Verify that seats can be selected without double booking.</t>
-  </si>
-  <si>
-    <t>Movie should be chosen and should be on booking page.</t>
-  </si>
-  <si>
-    <t>1. Movie and showtime must be selected.
-2. 3 seats must be chosen at different places across the theater.
-3. Another device to then attempt to pick the same seats.</t>
+    <t>AntiBot_1</t>
+  </si>
+  <si>
+    <t>Anti_botting_limitation</t>
   </si>
   <si>
     <t xml:space="preserve">The second device should not be able to pick those seats. </t>
@@ -158,13 +159,22 @@
     <t>Seats were not able to have been picked.</t>
   </si>
   <si>
-    <t>AntiBot_1</t>
-  </si>
-  <si>
-    <t>Anti_botting_limitation</t>
-  </si>
-  <si>
     <t>Verify that per-user ticket sales are limited to prevent botting/scalping practices</t>
+  </si>
+  <si>
+    <t>HotShow_1</t>
+  </si>
+  <si>
+    <t>Trending_Show_Display</t>
+  </si>
+  <si>
+    <t>P7</t>
+  </si>
+  <si>
+    <t>Verify that most trending shows are displayed on bar.</t>
+  </si>
+  <si>
+    <t>Site is already open.</t>
   </si>
   <si>
     <t>Generic customer account logged in, on any movie page</t>
@@ -186,19 +196,9 @@
 purchasing before the 10 purchases can be completed.</t>
   </si>
   <si>
-    <t>HotShow_1</t>
-  </si>
-  <si>
-    <t>Trending_Show_Display</t>
-  </si>
-  <si>
-    <t>P7</t>
-  </si>
-  <si>
-    <t>Verify that most trending shows are displayed on bar.</t>
-  </si>
-  <si>
-    <t>Site is already open.</t>
+    <t>1. Movie and showtime must be selected.
+2. 3 seats must be chosen at different places across the theater.
+3. Another device to then attempt to pick the same seats.</t>
   </si>
   <si>
     <t>1. Create 5 trending shows on a database not in ordered view of their ratings.
@@ -280,10 +280,10 @@
 not.</t>
   </si>
   <si>
+    <t>Theater_Schedule_Edit</t>
+  </si>
+  <si>
     <t>TheaterScheduling_1</t>
-  </si>
-  <si>
-    <t>Theater_Schedule_Edit</t>
   </si>
   <si>
     <t>P3</t>
@@ -303,13 +303,16 @@
   </si>
   <si>
     <t>Scheduling fails, user is notified of schedule conflict (specifically indicating the time and movie from the first schedule addition).</t>
+  </si>
+  <si>
+    <t>TEST CASES</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -317,16 +320,43 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="16"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="22"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="16"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -334,18 +364,162 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -361,6 +535,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -680,347 +858,367 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4B6C189B-F05F-B148-8008-BD9FF600D7F2}">
-  <dimension ref="A2:J11"/>
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="A1:J11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E9" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="55" workbookViewId="0">
+      <selection activeCell="M4" sqref="M4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.95"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="13.875" customWidth="1"/>
-    <col min="2" max="2" width="21.5" customWidth="1"/>
+    <col min="1" max="1" width="22.33203125" customWidth="1"/>
+    <col min="2" max="2" width="26.6640625" customWidth="1"/>
     <col min="4" max="4" width="58.5" customWidth="1"/>
     <col min="5" max="5" width="45.5" customWidth="1"/>
     <col min="6" max="6" width="28" customWidth="1"/>
-    <col min="7" max="7" width="66.375" customWidth="1"/>
-    <col min="8" max="8" width="35.875" customWidth="1"/>
-    <col min="9" max="9" width="9"/>
-    <col min="10" max="10" width="16.125" customWidth="1"/>
-    <col min="11" max="11" width="12.125" customWidth="1"/>
+    <col min="7" max="7" width="66.33203125" customWidth="1"/>
+    <col min="8" max="8" width="35.83203125" customWidth="1"/>
+    <col min="10" max="10" width="24.33203125" customWidth="1"/>
+    <col min="11" max="11" width="12.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:10" ht="15.75">
-      <c r="A2" t="s">
+    <row r="1" spans="1:10" ht="29" x14ac:dyDescent="0.35">
+      <c r="A1" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="B1" s="7"/>
+      <c r="C1" s="7"/>
+      <c r="D1" s="7"/>
+      <c r="E1" s="7"/>
+      <c r="F1" s="7"/>
+      <c r="G1" s="7"/>
+      <c r="H1" s="7"/>
+      <c r="I1" s="7"/>
+      <c r="J1" s="8"/>
+    </row>
+    <row r="2" spans="1:10" ht="22" x14ac:dyDescent="0.3">
+      <c r="A2" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E2" t="s">
+      <c r="E2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F2" t="s">
+      <c r="F2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G2" t="s">
+      <c r="G2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H2" t="s">
+      <c r="H2" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I2" t="s">
+      <c r="I2" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J2" t="s">
+      <c r="J2" s="10" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="15.75">
-      <c r="A3" t="s">
+    <row r="3" spans="1:10" ht="46" x14ac:dyDescent="0.3">
+      <c r="A3" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="D3" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="E3" t="s">
+      <c r="E3" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F3" s="2" t="s">
+      <c r="F3" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="I3" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="J3" s="12" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" ht="345" x14ac:dyDescent="0.3">
+      <c r="A4" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="G3" t="s">
-        <v>16</v>
-      </c>
-      <c r="H3" t="s">
+      <c r="B4" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="I3" t="s">
+      <c r="C4" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D4" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="J3" t="s">
+      <c r="E4" s="2" t="s">
         <v>19</v>
       </c>
+      <c r="F4" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="G4" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="H4" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="I4" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="J4" s="12" t="s">
+        <v>32</v>
+      </c>
     </row>
-    <row r="4" spans="1:10" ht="169.5">
-      <c r="A4" t="s">
-        <v>20</v>
-      </c>
-      <c r="B4" t="s">
-        <v>21</v>
-      </c>
-      <c r="C4" t="s">
-        <v>12</v>
-      </c>
-      <c r="D4" t="s">
+    <row r="5" spans="1:10" ht="207" x14ac:dyDescent="0.3">
+      <c r="A5" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="F5" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="H5" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="I5" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="E4" t="s">
+      <c r="J5" s="12" t="s">
         <v>23</v>
       </c>
-      <c r="F4" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="G4" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="H4" s="2" t="s">
+    </row>
+    <row r="6" spans="1:10" ht="276" x14ac:dyDescent="0.3">
+      <c r="A6" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="C6" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="I4" t="s">
-        <v>18</v>
-      </c>
-      <c r="J4" t="s">
-        <v>27</v>
+      <c r="D6" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="F6" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="G6" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="H6" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="I6" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="J6" s="12" t="s">
+        <v>32</v>
       </c>
     </row>
-    <row r="5" spans="1:10" ht="108">
-      <c r="A5" t="s">
-        <v>28</v>
-      </c>
-      <c r="B5" t="s">
-        <v>29</v>
-      </c>
-      <c r="C5" t="s">
-        <v>30</v>
-      </c>
-      <c r="D5" t="s">
-        <v>31</v>
-      </c>
-      <c r="E5" t="s">
+    <row r="7" spans="1:10" ht="230" x14ac:dyDescent="0.3">
+      <c r="A7" s="11" t="s">
+        <v>38</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="F7" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="G7" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="H7" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="I7" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="J7" s="12" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" ht="161" x14ac:dyDescent="0.3">
+      <c r="A8" s="11" t="s">
+        <v>51</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="E8" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="F8" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="G8" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="H8" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="I8" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="J8" s="12" t="s">
         <v>32</v>
       </c>
-      <c r="F5" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="G5" t="s">
-        <v>34</v>
-      </c>
-      <c r="H5" t="s">
-        <v>35</v>
-      </c>
-      <c r="I5" t="s">
-        <v>18</v>
-      </c>
-      <c r="J5" t="s">
-        <v>19</v>
-      </c>
     </row>
-    <row r="6" spans="1:10" ht="123">
-      <c r="A6" t="s">
-        <v>36</v>
-      </c>
-      <c r="B6" t="s">
-        <v>37</v>
-      </c>
-      <c r="C6" t="s">
-        <v>30</v>
-      </c>
-      <c r="D6" t="s">
-        <v>38</v>
-      </c>
-      <c r="E6" t="s">
-        <v>39</v>
-      </c>
-      <c r="F6" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="G6" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="H6" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="I6" t="s">
-        <v>18</v>
-      </c>
-      <c r="J6" t="s">
-        <v>27</v>
+    <row r="9" spans="1:10" ht="207" x14ac:dyDescent="0.3">
+      <c r="A9" s="11" t="s">
+        <v>57</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="E9" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="F9" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="G9" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="H9" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="I9" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="J9" s="12" t="s">
+        <v>32</v>
       </c>
     </row>
-    <row r="7" spans="1:10" ht="108">
-      <c r="A7" t="s">
-        <v>43</v>
-      </c>
-      <c r="B7" t="s">
-        <v>44</v>
-      </c>
-      <c r="C7" t="s">
-        <v>45</v>
-      </c>
-      <c r="D7" t="s">
-        <v>46</v>
-      </c>
-      <c r="E7" t="s">
-        <v>47</v>
-      </c>
-      <c r="F7" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="G7" t="s">
-        <v>49</v>
-      </c>
-      <c r="H7" t="s">
-        <v>50</v>
-      </c>
-      <c r="I7" t="s">
-        <v>18</v>
-      </c>
-      <c r="J7" t="s">
-        <v>19</v>
+    <row r="10" spans="1:10" ht="207" x14ac:dyDescent="0.3">
+      <c r="A10" s="11" t="s">
+        <v>62</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="E10" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="F10" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="G10" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="H10" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="I10" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="J10" s="12" t="s">
+        <v>32</v>
       </c>
     </row>
-    <row r="8" spans="1:10" ht="92.25">
-      <c r="A8" t="s">
-        <v>51</v>
-      </c>
-      <c r="B8" t="s">
-        <v>52</v>
-      </c>
-      <c r="C8" t="s">
-        <v>30</v>
-      </c>
-      <c r="D8" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="E8" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="F8" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="G8" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="H8" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="I8" t="s">
-        <v>18</v>
-      </c>
-      <c r="J8" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" ht="92.25">
-      <c r="A9" t="s">
-        <v>57</v>
-      </c>
-      <c r="B9" t="s">
-        <v>21</v>
-      </c>
-      <c r="C9" t="s">
-        <v>30</v>
-      </c>
-      <c r="D9" t="s">
-        <v>58</v>
-      </c>
-      <c r="E9" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="F9" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="G9" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="H9" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="I9" t="s">
-        <v>18</v>
-      </c>
-      <c r="J9" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" ht="138.75">
-      <c r="A10" t="s">
-        <v>62</v>
-      </c>
-      <c r="B10" t="s">
-        <v>63</v>
-      </c>
-      <c r="C10" t="s">
-        <v>30</v>
-      </c>
-      <c r="D10" t="s">
-        <v>64</v>
-      </c>
-      <c r="E10" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="F10" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="G10" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="H10" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="I10" t="s">
-        <v>18</v>
-      </c>
-      <c r="J10" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" ht="108">
-      <c r="A11" t="s">
+    <row r="11" spans="1:10" ht="185" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A11" s="13" t="s">
+        <v>69</v>
+      </c>
+      <c r="B11" s="14" t="s">
         <v>68</v>
       </c>
-      <c r="B11" t="s">
-        <v>69</v>
-      </c>
-      <c r="C11" t="s">
+      <c r="C11" s="14" t="s">
         <v>70</v>
       </c>
-      <c r="D11" s="2" t="s">
+      <c r="D11" s="15" t="s">
         <v>71</v>
       </c>
-      <c r="E11" t="s">
+      <c r="E11" s="14" t="s">
         <v>72</v>
       </c>
-      <c r="F11" s="2" t="s">
+      <c r="F11" s="15" t="s">
         <v>73</v>
       </c>
-      <c r="G11" s="2" t="s">
+      <c r="G11" s="15" t="s">
         <v>74</v>
       </c>
-      <c r="H11" s="2" t="s">
+      <c r="H11" s="15" t="s">
         <v>74</v>
       </c>
-      <c r="I11" t="s">
-        <v>18</v>
-      </c>
-      <c r="J11" t="s">
-        <v>27</v>
+      <c r="I11" s="16" t="s">
+        <v>22</v>
+      </c>
+      <c r="J11" s="17" t="s">
+        <v>32</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <mergeCells count="1">
+    <mergeCell ref="A1:J1"/>
+  </mergeCells>
+  <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup scale="28" orientation="landscape" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>